<commit_message>
Amended DSR testthat script
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR.xlsx
+++ b/tests/testthat/testdata_DSR.xlsx
@@ -1711,7 +1711,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,21 +1810,6 @@
       </c>
       <c r="C4">
         <v>8970</v>
-      </c>
-      <c r="D4" s="18">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="18">
-        <v>-1</v>
-      </c>
-      <c r="F4" s="18">
-        <v>-1</v>
-      </c>
-      <c r="G4" s="18">
-        <v>-1</v>
-      </c>
-      <c r="H4" s="18">
-        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Roxygen documentation code, Means function & DSR error handling
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR.xlsx
+++ b/tests/testthat/testdata_DSR.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="40">
   <si>
     <t>0-4</t>
   </si>
@@ -121,21 +121,6 @@
     <t>dsr</t>
   </si>
   <si>
-    <t>lower95cl</t>
-  </si>
-  <si>
-    <t>upper95cl</t>
-  </si>
-  <si>
-    <t>lower998cl</t>
-  </si>
-  <si>
-    <t>upper998cl</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
     <t>testdata_tiny</t>
   </si>
   <si>
@@ -143,6 +128,27 @@
   </si>
   <si>
     <t>testdata_1976</t>
+  </si>
+  <si>
+    <t>lowercl</t>
+  </si>
+  <si>
+    <t>uppercl</t>
+  </si>
+  <si>
+    <t>confidence</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Dobson</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
+    <t>99.8%</t>
   </si>
 </sst>
 </file>
@@ -227,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -293,6 +299,12 @@
     <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -578,7 +590,7 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1146,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
         <v>0</v>
@@ -1148,7 +1160,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -1162,7 +1174,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
         <v>2</v>
@@ -1176,7 +1188,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
@@ -1190,7 +1202,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
@@ -1204,7 +1216,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
@@ -1218,7 +1230,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
@@ -1232,7 +1244,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -1246,7 +1258,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -1260,7 +1272,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -1274,7 +1286,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -1288,7 +1300,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -1302,7 +1314,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -1316,7 +1328,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
         <v>13</v>
@@ -1330,7 +1342,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
         <v>14</v>
@@ -1344,7 +1356,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
@@ -1358,7 +1370,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B56" t="s">
         <v>16</v>
@@ -1372,7 +1384,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
         <v>17</v>
@@ -1386,7 +1398,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -1674,7 +1686,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4">
         <v>82</v>
@@ -1708,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,13 +1731,14 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="18"/>
-    <col min="5" max="7" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>27</v>
@@ -1737,16 +1750,16 @@
         <v>29</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1768,11 +1781,11 @@
       <c r="F2" s="18">
         <v>1117.894091547925</v>
       </c>
-      <c r="G2" s="18">
-        <v>932.32878802199036</v>
-      </c>
-      <c r="H2" s="18">
-        <v>1162.0595999522059</v>
+      <c r="G2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1794,16 +1807,16 @@
       <c r="F3" s="18">
         <v>136.70882227251795</v>
       </c>
-      <c r="G3" s="18">
-        <v>76.36420357939879</v>
-      </c>
-      <c r="H3" s="18">
-        <v>153.00328948244763</v>
+      <c r="G3" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -1811,10 +1824,16 @@
       <c r="C4">
         <v>8970</v>
       </c>
+      <c r="G4" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>804</v>
@@ -1831,11 +1850,106 @@
       <c r="F5" s="18">
         <v>9225.2538803183179</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>895</v>
+      </c>
+      <c r="C6">
+        <v>8970</v>
+      </c>
+      <c r="D6" s="18">
+        <v>1043.0247991469423</v>
+      </c>
+      <c r="E6" s="18">
+        <v>932.32878802199036</v>
+      </c>
+      <c r="F6" s="18">
+        <v>1162.0595999522059</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>91</v>
+      </c>
+      <c r="C7">
+        <v>8970</v>
+      </c>
+      <c r="D7" s="18">
+        <v>110.3212025300104</v>
+      </c>
+      <c r="E7" s="18">
+        <v>76.36420357939879</v>
+      </c>
+      <c r="F7" s="18">
+        <v>153.00328948244763</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>8970</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>804</v>
+      </c>
+      <c r="C9">
+        <v>8763</v>
+      </c>
+      <c r="D9" s="18">
+        <v>8592.0975850223658</v>
+      </c>
+      <c r="E9" s="18">
         <v>7659.2821065689559</v>
       </c>
-      <c r="H5" s="18">
+      <c r="F9" s="18">
         <v>9599.2117985716977</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
amended DSR function and test script - 2 error checks still to add
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR.xlsx
+++ b/tests/testthat/testdata_DSR.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="45">
   <si>
     <t>0-4</t>
   </si>
@@ -149,6 +149,21 @@
   </si>
   <si>
     <t>99.8%</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>dsr per 100000</t>
+  </si>
+  <si>
+    <t>dsr per 10000</t>
+  </si>
+  <si>
+    <t>NA - total count is &lt; 10</t>
   </si>
 </sst>
 </file>
@@ -590,7 +605,7 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,10 +1748,11 @@
     <col min="4" max="4" width="9.140625" style="18"/>
     <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="23" customWidth="1"/>
+    <col min="9" max="9" width="11" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -1758,11 +1774,17 @@
       <c r="G1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1784,11 +1806,17 @@
       <c r="G2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1810,11 +1838,17 @@
       <c r="G3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1824,14 +1858,29 @@
       <c r="C4">
         <v>8970</v>
       </c>
+      <c r="D4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="G4" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1853,11 +1902,17 @@
       <c r="G5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1879,11 +1934,17 @@
       <c r="G6" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1905,11 +1966,17 @@
       <c r="G7" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1919,14 +1986,29 @@
       <c r="C8">
         <v>8970</v>
       </c>
+      <c r="D8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="G8" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1948,8 +2030,288 @@
       <c r="G9" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>37</v>
+      </c>
+      <c r="J9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>895</v>
+      </c>
+      <c r="C10">
+        <v>8970</v>
+      </c>
+      <c r="D10" s="18">
+        <f>D2*10</f>
+        <v>10430.247991469423</v>
+      </c>
+      <c r="E10" s="18">
+        <f t="shared" ref="E10:F10" si="0">E2*10</f>
+        <v>9717.709067985681</v>
+      </c>
+      <c r="F10" s="18">
+        <f t="shared" si="0"/>
+        <v>11178.94091547925</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>91</v>
+      </c>
+      <c r="C11">
+        <v>8970</v>
+      </c>
+      <c r="D11" s="18">
+        <f t="shared" ref="D11:F11" si="1">D3*10</f>
+        <v>1103.212025300104</v>
+      </c>
+      <c r="E11" s="18">
+        <f t="shared" si="1"/>
+        <v>877.455767536709</v>
+      </c>
+      <c r="F11" s="18">
+        <f t="shared" si="1"/>
+        <v>1367.0882227251795</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>8970</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>804</v>
+      </c>
+      <c r="C13">
+        <v>8763</v>
+      </c>
+      <c r="D13" s="18">
+        <f t="shared" ref="D13:F13" si="2">D5*10</f>
+        <v>85920.975850223651</v>
+      </c>
+      <c r="E13" s="18">
+        <f t="shared" si="2"/>
+        <v>79911.609314421032</v>
+      </c>
+      <c r="F13" s="18">
+        <f t="shared" si="2"/>
+        <v>92252.538803183183</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>895</v>
+      </c>
+      <c r="C14">
+        <v>8970</v>
+      </c>
+      <c r="D14" s="18">
+        <f t="shared" ref="D14:F14" si="3">D6*10</f>
+        <v>10430.247991469423</v>
+      </c>
+      <c r="E14" s="18">
+        <f t="shared" si="3"/>
+        <v>9323.2878802199029</v>
+      </c>
+      <c r="F14" s="18">
+        <f t="shared" si="3"/>
+        <v>11620.595999522058</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>8970</v>
+      </c>
+      <c r="D15" s="18">
+        <f t="shared" ref="D15:F15" si="4">D7*10</f>
+        <v>1103.212025300104</v>
+      </c>
+      <c r="E15" s="18">
+        <f t="shared" si="4"/>
+        <v>763.64203579398793</v>
+      </c>
+      <c r="F15" s="18">
+        <f t="shared" si="4"/>
+        <v>1530.0328948244762</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>8970</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>804</v>
+      </c>
+      <c r="C17">
+        <v>8763</v>
+      </c>
+      <c r="D17" s="18">
+        <f t="shared" ref="D17:F17" si="5">D9*10</f>
+        <v>85920.975850223651</v>
+      </c>
+      <c r="E17" s="18">
+        <f t="shared" si="5"/>
+        <v>76592.821065689554</v>
+      </c>
+      <c r="F17" s="18">
+        <f t="shared" si="5"/>
+        <v>95992.117985716977</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -2584,7 +2946,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>